<commit_message>
Add Excel Sheet to Data Source
</commit_message>
<xml_diff>
--- a/All Users.xlsx
+++ b/All Users.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHATHURI\Documents\SOAPUI\Automation Assignment\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -54,6 +54,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>

</xml_diff>

<commit_message>
Add Data Sink Option
</commit_message>
<xml_diff>
--- a/All Users.xlsx
+++ b/All Users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHATHURI\Documents\SOAPUI\Automation Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E163A95-8DDF-40A8-B6C9-E1F55DC3C81F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245756D6-6226-4358-82D3-A112D8E530BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3015" yWindow="2175" windowWidth="21600" windowHeight="11505" xr2:uid="{E6FB995B-1F50-49A0-AAC5-6C177AF09FD5}"/>
+    <workbookView xWindow="2670" yWindow="1830" windowWidth="21600" windowHeight="11505" xr2:uid="{E6FB995B-1F50-49A0-AAC5-6C177AF09FD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,21 +33,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Id</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>Avatar</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Job</t>
+  </si>
+  <si>
+    <t>470</t>
+  </si>
+  <si>
+    <t>Engineer</t>
+  </si>
+  <si>
+    <t>&lt;job xmlns="https://reqres.in/api/users"/&gt;</t>
+  </si>
+  <si>
+    <t>398</t>
+  </si>
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Doctor</t>
+  </si>
+  <si>
+    <t>318</t>
+  </si>
+  <si>
+    <t>chathuri</t>
+  </si>
+  <si>
+    <t>542</t>
+  </si>
+  <si>
+    <t>buddhika</t>
+  </si>
+  <si>
+    <t>865</t>
+  </si>
+  <si>
+    <t>gunapala</t>
   </si>
 </sst>
 </file>
@@ -400,15 +433,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97641834-A8B5-456C-ABB5-388031B8859D}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -418,11 +451,71 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B2" t="s">
         <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>